<commit_message>
Implement IFF (bug with negated if)
</commit_message>
<xml_diff>
--- a/documents/GanttChart.xlsx
+++ b/documents/GanttChart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{628FA0F1-3BA1-4679-A346-27EA6A5E624E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B82D034B-4A75-4D6E-B193-6D5881A03AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Task 3</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Avoid Refutation Proofs</t>
   </si>
   <si>
-    <t>Extend Natural Language Argumentation</t>
-  </si>
-  <si>
     <t>Flexibilize Conditional Sentences order</t>
   </si>
   <si>
@@ -251,6 +248,15 @@
   </si>
   <si>
     <t>Arbitrary verb in syllogisms</t>
+  </si>
+  <si>
+    <t>Natural Language Argumentation</t>
+  </si>
+  <si>
+    <t>Propositional and Predicate Logic</t>
+  </si>
+  <si>
+    <t>Defeasible Logic</t>
   </si>
 </sst>
 </file>
@@ -1494,8 +1500,8 @@
   <dimension ref="A1:BL36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2273,7 +2279,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="76" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="68" t="s">
         <v>31</v>
@@ -2354,7 +2360,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="68"/>
       <c r="D10" s="22">
@@ -2431,7 +2437,7 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="58"/>
       <c r="B11" s="76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="68"/>
       <c r="D11" s="22">
@@ -3086,7 +3092,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C20" s="71"/>
       <c r="D20" s="29"/>
@@ -3157,7 +3163,7 @@
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="58"/>
       <c r="B21" s="78" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="C21" s="72"/>
       <c r="D21" s="32"/>
@@ -3234,7 +3240,7 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="58"/>
       <c r="B22" s="78" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C22" s="72"/>
       <c r="D22" s="32"/>
@@ -3544,7 +3550,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="73"/>
       <c r="D26" s="34"/>
@@ -3615,7 +3621,7 @@
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="58"/>
       <c r="B27" s="79" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="74"/>
       <c r="D27" s="37">
@@ -3692,7 +3698,7 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="58"/>
       <c r="B28" s="79" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="74"/>
       <c r="D28" s="37"/>
@@ -3767,7 +3773,7 @@
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="58"/>
       <c r="B29" s="79" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="74"/>
       <c r="D29" s="37"/>

</xml_diff>